<commit_message>
Added sidebar and bar style
</commit_message>
<xml_diff>
--- a/Planung/GantChart.xlsx
+++ b/Planung/GantChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Desktop\IMS-T\IP\Projekte\Carsdex\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC87F364-B1D1-4873-A4A8-B816375FE6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE14801F-1159-4881-926A-3D6B7B65A942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16FFFFC1-273D-404B-811D-5FED091368E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{16FFFFC1-273D-404B-811D-5FED091368E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Gantt Chart Carsdex</t>
   </si>
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -257,6 +257,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -266,13 +275,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +615,7 @@
   <dimension ref="A1:AX28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI9" sqref="AI9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,110 +627,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="15"/>
+      <c r="AK1" s="15"/>
+      <c r="AL1" s="15"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="15"/>
+      <c r="AO1" s="15"/>
+      <c r="AP1" s="15"/>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="12"/>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
+      <c r="AF2" s="15"/>
+      <c r="AG2" s="15"/>
+      <c r="AH2" s="15"/>
+      <c r="AI2" s="15"/>
+      <c r="AJ2" s="15"/>
+      <c r="AK2" s="15"/>
+      <c r="AL2" s="15"/>
+      <c r="AM2" s="15"/>
+      <c r="AN2" s="15"/>
+      <c r="AO2" s="15"/>
+      <c r="AP2" s="15"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="15"/>
+      <c r="AS2" s="15"/>
+      <c r="AT2" s="15"/>
+      <c r="AU2" s="15"/>
+      <c r="AV2" s="15"/>
+      <c r="AW2" s="15"/>
+      <c r="AX2" s="15"/>
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -882,15 +885,15 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="Q4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="AT4" s="14" t="s">
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="AT4" s="17" t="s">
         <v>26</v>
       </c>
       <c r="AX4" s="2"/>
@@ -900,16 +903,16 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="AT5" s="14"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="AT5" s="17"/>
       <c r="AX5" s="2"/>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
@@ -917,14 +920,14 @@
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="AT6" s="14"/>
+      <c r="C6" s="12"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="AT6" s="17"/>
       <c r="AX6" s="2"/>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
@@ -932,16 +935,22 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="AT7" s="14"/>
+      <c r="F7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="AT7" s="17"/>
       <c r="AX7" s="2"/>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
@@ -951,13 +960,13 @@
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="AT8" s="14"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="AT8" s="17"/>
       <c r="AX8" s="2"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
@@ -965,16 +974,16 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="AT9" s="14"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="AT9" s="17"/>
       <c r="AX9" s="2"/>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
@@ -982,13 +991,13 @@
       <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="AT10" s="14"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="AT10" s="17"/>
       <c r="AX10" s="2"/>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
@@ -996,16 +1005,16 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="AT11" s="14"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="AT11" s="17"/>
       <c r="AX11" s="2"/>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
@@ -1013,14 +1022,16 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="AT12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="16"/>
+      <c r="AT12" s="17"/>
       <c r="AX12" s="2"/>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
@@ -1028,13 +1039,13 @@
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="AT13" s="14"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="16"/>
+      <c r="AT13" s="17"/>
       <c r="AX13" s="2"/>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
@@ -1042,13 +1053,13 @@
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="AT14" s="14"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="16"/>
+      <c r="AT14" s="17"/>
       <c r="AX14" s="2"/>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
@@ -1062,13 +1073,13 @@
       <c r="N15" s="8"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="AT15" s="14"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="16"/>
+      <c r="AT15" s="17"/>
       <c r="AX15" s="2"/>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
@@ -1076,17 +1087,17 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="16"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
-      <c r="AT16" s="14"/>
+      <c r="AT16" s="17"/>
       <c r="AX16" s="2"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
@@ -1094,16 +1105,16 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="16"/>
+      <c r="S17" s="16"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="16"/>
+      <c r="V17" s="16"/>
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
       <c r="AC17" s="8"/>
-      <c r="AT17" s="14"/>
+      <c r="AT17" s="17"/>
       <c r="AX17" s="2"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
@@ -1111,13 +1122,13 @@
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="AT18" s="14"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="16"/>
+      <c r="AT18" s="17"/>
       <c r="AX18" s="2"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
@@ -1125,17 +1136,17 @@
       <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="16"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="16"/>
+      <c r="V19" s="16"/>
       <c r="AD19" s="9"/>
       <c r="AE19" s="9"/>
       <c r="AF19" s="9"/>
       <c r="AG19" s="9"/>
-      <c r="AT19" s="14"/>
+      <c r="AT19" s="17"/>
       <c r="AX19" s="2"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
@@ -1143,15 +1154,15 @@
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
       <c r="AH20" s="9"/>
       <c r="AI20" s="9"/>
-      <c r="AT20" s="14"/>
+      <c r="AT20" s="17"/>
       <c r="AX20" s="2"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
@@ -1159,12 +1170,12 @@
       <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="16"/>
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
       <c r="AJ21" s="4"/>
       <c r="AK21" s="4"/>
       <c r="AL21" s="4"/>
@@ -1174,7 +1185,7 @@
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
       <c r="AR21" s="4"/>
-      <c r="AT21" s="14"/>
+      <c r="AT21" s="17"/>
       <c r="AX21" s="2"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
@@ -1182,14 +1193,14 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
       <c r="AS22" s="4"/>
-      <c r="AT22" s="14"/>
+      <c r="AT22" s="17"/>
       <c r="AU22" s="4"/>
       <c r="AX22" s="2"/>
     </row>
@@ -1198,13 +1209,13 @@
       <c r="B23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="AT23" s="14"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="AT23" s="17"/>
       <c r="AX23" s="2"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
@@ -1212,13 +1223,13 @@
       <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="AT24" s="14"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="AT24" s="17"/>
       <c r="AU24" s="5"/>
       <c r="AX24" s="2"/>
     </row>
@@ -1227,13 +1238,13 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="AT25" s="14"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="AT25" s="17"/>
       <c r="AU25" s="5"/>
       <c r="AX25" s="2"/>
     </row>
@@ -1242,13 +1253,13 @@
       <c r="B26" t="s">
         <v>23</v>
       </c>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="AT26" s="14"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="AT26" s="17"/>
       <c r="AV26" s="5"/>
       <c r="AW26" s="5"/>
       <c r="AX26" s="2"/>

</xml_diff>